<commit_message>
Fehler versucht zu beheben
zugelabert worden
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Webseiten\Abschlussprojekt\Schiffe-versenken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2D7810-B0D4-4370-808D-5122A2FE6E82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B50A51-86E5-4FF6-BE46-62BE52CB2AEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{B588D240-05C9-4689-9B05-EEA7D26A57F2}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="12">
-        <v>0.66666666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="D7" s="12">
         <v>0.66666666666666663</v>
@@ -642,7 +642,7 @@
       </c>
       <c r="C8" s="4">
         <f>C7-C6-C9</f>
-        <v>0.29166666666666663</v>
+        <v>0.3125</v>
       </c>
       <c r="D8" s="4">
         <f>D7-D6-D9</f>
@@ -662,7 +662,7 @@
       </c>
       <c r="H8" s="3">
         <f>SUM(C8:G8)*24</f>
-        <v>34</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="3">
         <f>H16+H8+H12+H4</f>
-        <v>77.75</v>
+        <v>78.25</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>